<commit_message>
feat: Implement expense management features including adding, deleting, and downloading expenses
- Added AddExpenseForm component for adding new expenses.
- Implemented ExpenseList component to display and manage expenses.
- Created ExpenseOverview component to visualize expense trends with a line chart.
- Integrated CustomLineChart for displaying expense data.
- Enhanced API paths for expense-related operations.
- Updated helper functions to prepare data for charts.
- Added modal functionality for adding and deleting expenses.
- Improved UI components for better user experience.
- Added functionality to download expense details as an Excel file.
</commit_message>
<xml_diff>
--- a/server/expense_details.xlsx
+++ b/server/expense_details.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -417,7 +417,7 @@
       <c r="A2" t="str">
         <v>Food</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B2">
         <v>1000</v>
       </c>
       <c r="C2" t="str">
@@ -428,7 +428,7 @@
       <c r="A3" t="str">
         <v>Travel</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B3">
         <v>12000</v>
       </c>
       <c r="C3" t="str">
@@ -439,7 +439,7 @@
       <c r="A4" t="str">
         <v>Books</v>
       </c>
-      <c r="B4" t="str">
+      <c r="B4">
         <v>2000</v>
       </c>
       <c r="C4" t="str">
@@ -450,16 +450,71 @@
       <c r="A5" t="str">
         <v>testing-2</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B5">
         <v>2000</v>
       </c>
       <c r="C5" t="str">
         <v>2025-09-19</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>shopping</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2025-11-09</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>movies</v>
+      </c>
+      <c r="B7">
+        <v>2000</v>
+      </c>
+      <c r="C7" t="str">
+        <v>2025-11-09</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>groceries</v>
+      </c>
+      <c r="B8">
+        <v>1200</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2025-11-09</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Rent</v>
+      </c>
+      <c r="B9">
+        <v>10000</v>
+      </c>
+      <c r="C9" t="str">
+        <v>2025-11-10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Groceries</v>
+      </c>
+      <c r="B10">
+        <v>2000</v>
+      </c>
+      <c r="C10" t="str">
+        <v>2025-11-08</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>